<commit_message>
Inserindo limite opcional para geração de cartazes. | Formulário para cartazes únicos criado.
</commit_message>
<xml_diff>
--- a/PosterMailer-front-end/public/assets/sheets/modelo-cartaz.xlsx
+++ b/PosterMailer-front-end/public/assets/sheets/modelo-cartaz.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Produto</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>Preco</t>
+  </si>
+  <si>
+    <t>Limite</t>
   </si>
   <si>
     <t>;</t>
@@ -38,9 +41,9 @@
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -50,7 +53,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -107,9 +109,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -158,7 +157,10 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -169,12 +171,7 @@
     <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -394,7 +391,8 @@
     <col customWidth="1" min="1" max="1" width="53.57"/>
     <col customWidth="1" min="2" max="2" width="10.14"/>
     <col customWidth="1" min="3" max="3" width="11.29"/>
-    <col customWidth="1" min="4" max="6" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="8.14"/>
+    <col customWidth="1" min="5" max="6" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -407,25 +405,31 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="9">
       <c r="P9" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>